<commit_message>
Update Cypress tests, configs, TestCase.xlsx; remove unused files
</commit_message>
<xml_diff>
--- a/Manual Testing/TestCase.xlsx
+++ b/Manual Testing/TestCase.xlsx
@@ -1,28 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\QA-Manual-and-Automation-Testing\Manual Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7D0080-633C-4770-A2AB-A7ECE5DC1081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AC1A04-5F1D-4E07-B35D-B2F3C289C1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" Test Cases Template" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="138">
   <si>
     <t>Manual Test Case Template – Search &amp; Filter Feature</t>
   </si>
@@ -478,6 +490,39 @@
   </si>
   <si>
     <t>Admin user is logged in and navigated to Add Employee page.</t>
+  </si>
+  <si>
+    <t>User was successfully logged in and redirected to the Dashboard page.</t>
+  </si>
+  <si>
+    <t>System displayed a warning message “Invalid credentials” and prevented login.</t>
+  </si>
+  <si>
+    <t>User was successfully logged out and redirected to the login page.</t>
+  </si>
+  <si>
+    <t>New employee “WadhaAlgarni2” was successfully created and appeared in the Employee List.</t>
+  </si>
+  <si>
+    <t>Employee record for “WadhaAlgarni2” appeared in the Employee List with correct details.</t>
+  </si>
+  <si>
+    <t>System displayed validation messages for required fields and did not create a new record.</t>
+  </si>
+  <si>
+    <t>Personal details were successfully updated and saved in the system.</t>
+  </si>
+  <si>
+    <t>Profile image was successfully uploaded and updated on the user profile.</t>
+  </si>
+  <si>
+    <t>System displayed an error “Job Title already exists” and did not save the duplicate job.</t>
+  </si>
+  <si>
+    <t>Job “Software Engineer - QA” was successfully added and appeared in the Job Titles list.</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -879,7 +924,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -912,6 +957,31 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -960,73 +1030,44 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1283,165 +1324,165 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="28" x14ac:dyDescent="0.75">
-      <c r="A1" s="13"/>
-      <c r="B1" s="24" t="s">
+      <c r="A1" s="22"/>
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="20"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="29"/>
     </row>
     <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.5">
-      <c r="A2" s="14"/>
-      <c r="B2" s="21" t="s">
+      <c r="A2" s="23"/>
+      <c r="B2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="17"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="26"/>
     </row>
     <row r="3" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="36" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="22" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="17"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="26"/>
     </row>
     <row r="4" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="17"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="26"/>
     </row>
     <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.5">
-      <c r="A5" s="14"/>
-      <c r="B5" s="37" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="17"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="26"/>
     </row>
     <row r="6" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="35" t="s">
+      <c r="A6" s="23"/>
+      <c r="B6" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="35" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="28">
         <v>45860</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="17"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="26"/>
     </row>
     <row r="7" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="17"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="26"/>
     </row>
     <row r="8" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="14"/>
-      <c r="B8" s="37" t="s">
+      <c r="A8" s="23"/>
+      <c r="B8" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="17"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="26"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="14"/>
-      <c r="B9" s="23" t="s">
+      <c r="A9" s="23"/>
+      <c r="B9" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="17"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="26"/>
     </row>
     <row r="10" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="14"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
@@ -1472,10 +1513,10 @@
       <c r="K10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="17"/>
+      <c r="L10" s="26"/>
     </row>
     <row r="11" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="14"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="5" t="s">
         <v>25</v>
       </c>
@@ -1504,10 +1545,10 @@
         <v>33</v>
       </c>
       <c r="K11" s="5"/>
-      <c r="L11" s="17"/>
+      <c r="L11" s="26"/>
     </row>
     <row r="12" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="14"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
@@ -1536,10 +1577,10 @@
         <v>38</v>
       </c>
       <c r="K12" s="5"/>
-      <c r="L12" s="17"/>
+      <c r="L12" s="26"/>
     </row>
     <row r="13" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="14"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="5" t="s">
         <v>39</v>
       </c>
@@ -1568,77 +1609,77 @@
         <v>38</v>
       </c>
       <c r="K13" s="5"/>
-      <c r="L13" s="17"/>
+      <c r="L13" s="26"/>
     </row>
     <row r="14" spans="1:12" ht="15.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="14"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="17"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="26"/>
     </row>
     <row r="15" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="17"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="26"/>
     </row>
     <row r="16" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="17"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="26"/>
     </row>
     <row r="17" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="17"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="26"/>
     </row>
     <row r="18" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="17"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -1668,13 +1709,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F0D7D9-DA37-4031-B40D-BD7FBDA20576}">
   <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="39" zoomScaleNormal="44" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C14"/>
+    <sheetView tabSelected="1" topLeftCell="E25" zoomScale="44" zoomScaleNormal="44" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.81640625" style="48" customWidth="1"/>
+    <col min="1" max="1" width="38.81640625" style="7" customWidth="1"/>
     <col min="2" max="2" width="18.26953125" style="7" customWidth="1"/>
     <col min="3" max="3" width="41.36328125" style="7" customWidth="1"/>
     <col min="4" max="4" width="21.453125" style="7" customWidth="1"/>
@@ -1683,9 +1724,9 @@
     <col min="7" max="7" width="48.81640625" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.54296875" style="7" customWidth="1"/>
     <col min="9" max="9" width="70.453125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="20.36328125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="96.54296875" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.6328125" style="7" customWidth="1"/>
-    <col min="12" max="12" width="37.81640625" style="48" customWidth="1"/>
+    <col min="12" max="12" width="37.81640625" style="7" customWidth="1"/>
     <col min="14" max="21" width="8.7265625" style="7"/>
     <col min="22" max="22" width="1.7265625" style="7" customWidth="1"/>
     <col min="23" max="25" width="8.7265625" style="7" hidden="1" customWidth="1"/>
@@ -1695,156 +1736,155 @@
   <sheetData>
     <row r="1" spans="1:12" ht="47.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
       <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:12" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52" t="s">
+      <c r="C2" s="56"/>
+      <c r="D2" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="52"/>
+      <c r="E2" s="53"/>
       <c r="L2" s="8"/>
     </row>
     <row r="3" spans="1:12" ht="48.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="53" t="s">
+      <c r="C3" s="56"/>
+      <c r="D3" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="52"/>
+      <c r="E3" s="53"/>
       <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="52">
+      <c r="C4" s="56"/>
+      <c r="D4" s="53">
         <v>1</v>
       </c>
-      <c r="E4" s="52"/>
+      <c r="E4" s="53"/>
       <c r="L4" s="8"/>
     </row>
     <row r="5" spans="1:12" ht="45.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="54">
+      <c r="C5" s="56"/>
+      <c r="D5" s="55">
         <v>45910</v>
       </c>
-      <c r="E5" s="54"/>
-      <c r="F5" s="40"/>
+      <c r="E5" s="55"/>
       <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="53" t="s">
+      <c r="C6" s="56"/>
+      <c r="D6" s="54" t="s">
         <v>114</v>
       </c>
-      <c r="E6" s="52"/>
+      <c r="E6" s="53"/>
       <c r="L6" s="8"/>
     </row>
     <row r="7" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="52" t="s">
+      <c r="C7" s="56"/>
+      <c r="D7" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="52"/>
+      <c r="E7" s="53"/>
       <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="52" t="s">
+      <c r="C8" s="56"/>
+      <c r="D8" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="52"/>
+      <c r="E8" s="53"/>
       <c r="L8" s="8"/>
     </row>
     <row r="9" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="C9" s="41"/>
+      <c r="C9" s="13"/>
       <c r="L9" s="8"/>
     </row>
-    <row r="10" spans="1:12" s="46" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
-      <c r="B10" s="44" t="s">
+    <row r="10" spans="1:12" s="18" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="44" t="s">
+      <c r="F10" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="45" t="s">
+      <c r="G10" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="45" t="s">
+      <c r="H10" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="44" t="s">
+      <c r="I10" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="44" t="s">
+      <c r="J10" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="K10" s="44" t="s">
+      <c r="K10" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="L10" s="43"/>
+      <c r="L10" s="15"/>
     </row>
     <row r="11" spans="1:12" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="55" t="s">
+      <c r="C11" s="48" t="s">
         <v>73</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="14" t="s">
         <v>71</v>
       </c>
       <c r="F11" s="9" t="s">
@@ -1856,11 +1896,15 @@
       <c r="H11" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="42" t="s">
+      <c r="I11" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
+      <c r="J11" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>137</v>
+      </c>
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:12" ht="46.5" x14ac:dyDescent="0.25">
@@ -1868,11 +1912,11 @@
       <c r="B12" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="56"/>
+      <c r="C12" s="52"/>
       <c r="D12" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="14" t="s">
         <v>71</v>
       </c>
       <c r="F12" s="9" t="s">
@@ -1884,11 +1928,15 @@
       <c r="H12" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="42" t="s">
+      <c r="I12" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
+      <c r="J12" s="59" t="s">
+        <v>128</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>137</v>
+      </c>
       <c r="L12" s="8"/>
     </row>
     <row r="13" spans="1:12" ht="46.5" x14ac:dyDescent="0.25">
@@ -1896,11 +1944,11 @@
       <c r="B13" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="56"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="14" t="s">
         <v>71</v>
       </c>
       <c r="F13" s="9" t="s">
@@ -1912,11 +1960,15 @@
       <c r="H13" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="I13" s="42" t="s">
+      <c r="I13" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
+      <c r="J13" s="59" t="s">
+        <v>128</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>137</v>
+      </c>
       <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:12" ht="46.5" x14ac:dyDescent="0.25">
@@ -1924,11 +1976,11 @@
       <c r="B14" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="57"/>
+      <c r="C14" s="49"/>
       <c r="D14" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="14" t="s">
         <v>71</v>
       </c>
       <c r="F14" s="9" t="s">
@@ -1940,11 +1992,15 @@
       <c r="H14" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="I14" s="42" t="s">
+      <c r="I14" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
+      <c r="J14" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>137</v>
+      </c>
       <c r="L14" s="8"/>
     </row>
     <row r="15" spans="1:12" ht="46.5" x14ac:dyDescent="0.25">
@@ -1952,13 +2008,13 @@
       <c r="B15" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="58" t="s">
+      <c r="C15" s="21" t="s">
         <v>80</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="14" t="s">
         <v>83</v>
       </c>
       <c r="F15" s="9" t="s">
@@ -1973,8 +2029,12 @@
       <c r="I15" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
+      <c r="J15" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>137</v>
+      </c>
       <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12" ht="155" x14ac:dyDescent="0.25">
@@ -1982,13 +2042,13 @@
       <c r="B16" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="59" t="s">
+      <c r="C16" s="47" t="s">
         <v>82</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="14" t="s">
         <v>119</v>
       </c>
       <c r="F16" s="9" t="s">
@@ -2000,11 +2060,15 @@
       <c r="H16" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I16" s="42" t="s">
+      <c r="I16" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
+      <c r="J16" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>137</v>
+      </c>
       <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:13" ht="62" x14ac:dyDescent="0.25">
@@ -2012,11 +2076,11 @@
       <c r="B17" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="59"/>
+      <c r="C17" s="47"/>
       <c r="D17" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="14" t="s">
         <v>125</v>
       </c>
       <c r="F17" s="9" t="s">
@@ -2028,11 +2092,15 @@
       <c r="H17" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="I17" s="42" t="s">
+      <c r="I17" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
+      <c r="J17" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>137</v>
+      </c>
       <c r="L17" s="8"/>
     </row>
     <row r="18" spans="1:13" ht="93" x14ac:dyDescent="0.25">
@@ -2040,14 +2108,14 @@
       <c r="B18" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="59"/>
+      <c r="C18" s="47"/>
       <c r="D18" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="F18" s="42" t="s">
+      <c r="F18" s="14" t="s">
         <v>115</v>
       </c>
       <c r="G18" s="11" t="s">
@@ -2056,11 +2124,15 @@
       <c r="H18" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="I18" s="42" t="s">
+      <c r="I18" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
+      <c r="J18" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>137</v>
+      </c>
       <c r="L18" s="8"/>
     </row>
     <row r="19" spans="1:13" ht="139.5" x14ac:dyDescent="0.25">
@@ -2068,13 +2140,13 @@
       <c r="B19" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="55" t="s">
+      <c r="C19" s="48" t="s">
         <v>88</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="14" t="s">
         <v>81</v>
       </c>
       <c r="F19" s="9" t="s">
@@ -2089,8 +2161,12 @@
       <c r="I19" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
+      <c r="J19" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>137</v>
+      </c>
       <c r="L19" s="8"/>
     </row>
     <row r="20" spans="1:13" ht="139.5" x14ac:dyDescent="0.25">
@@ -2098,11 +2174,11 @@
       <c r="B20" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="57"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="E20" s="14" t="s">
         <v>102</v>
       </c>
       <c r="F20" s="9" t="s">
@@ -2114,22 +2190,26 @@
       <c r="H20" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="I20" s="42" t="s">
+      <c r="I20" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
+      <c r="J20" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>137</v>
+      </c>
       <c r="L20" s="8"/>
     </row>
     <row r="21" spans="1:13" ht="62" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="60" t="s">
+      <c r="C21" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="47" t="s">
+      <c r="D21" s="19" t="s">
         <v>70</v>
       </c>
       <c r="E21" s="7" t="s">
@@ -2147,8 +2227,12 @@
       <c r="I21" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
+      <c r="J21" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>137</v>
+      </c>
       <c r="L21" s="8"/>
     </row>
     <row r="22" spans="1:13" ht="124" x14ac:dyDescent="0.25">
@@ -2156,14 +2240,14 @@
       <c r="B22" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="61"/>
+      <c r="C22" s="51"/>
       <c r="D22" s="9" t="s">
         <v>70</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="F22" s="42" t="s">
+      <c r="F22" s="14" t="s">
         <v>117</v>
       </c>
       <c r="G22" s="11" t="s">
@@ -2175,9 +2259,13 @@
       <c r="I22" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="50"/>
+      <c r="J22" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="L22" s="20"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D23" s="10"/>
@@ -2191,7 +2279,7 @@
       <c r="E24" s="10"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
-      <c r="L24" s="49"/>
+      <c r="L24"/>
       <c r="M24" s="7"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2200,14 +2288,14 @@
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
       <c r="I25"/>
-      <c r="L25" s="49"/>
+      <c r="L25"/>
       <c r="M25" s="7"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E26" s="10"/>
       <c r="G26" s="7"/>
       <c r="J26"/>
-      <c r="L26" s="49"/>
+      <c r="L26"/>
       <c r="M26" s="7"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -2217,6 +2305,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C21:C22"/>
@@ -2230,11 +2323,6 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>

</xml_diff>